<commit_message>
Cost Of Living for all years
</commit_message>
<xml_diff>
--- a/data/CostOfLivingProcessed.xlsx
+++ b/data/CostOfLivingProcessed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19344" windowHeight="9168" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19344" windowHeight="9168"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="2" r:id="rId1"/>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6858,7 +6858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>